<commit_message>
excel is added with data
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\pos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suchitra\git\pos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48587FD-312F-4FC0-904A-BEEBBCC8A771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -30,19 +29,19 @@
     <t>admin</t>
   </si>
   <si>
-    <t>pointofsale</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
     <t>Password</t>
   </si>
+  <si>
+    <t>pointofsale1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,32 +352,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>